<commit_message>
Update Bike Charging stations features.xlsx
</commit_message>
<xml_diff>
--- a/Bike Charging stations features.xlsx
+++ b/Bike Charging stations features.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wajiz.pk\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABC\Documents\GitHub\Electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10710" windowHeight="4100" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10710" windowHeight="4095" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bike features" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>Bike Application Pending/In process/completed task</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Card Swipping Management</t>
+  </si>
+  <si>
+    <t>Processing</t>
   </si>
 </sst>
 </file>
@@ -521,14 +524,14 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -539,7 +542,7 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -553,19 +556,19 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="7"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -576,7 +579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -587,7 +590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -598,7 +601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -609,7 +612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -620,7 +623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -634,7 +637,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -648,7 +651,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -659,7 +662,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -673,7 +676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -684,7 +687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>11</v>
       </c>
@@ -695,7 +698,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>12</v>
       </c>
@@ -709,7 +712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>13</v>
       </c>
@@ -720,7 +723,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -731,7 +734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>15</v>
       </c>
@@ -754,20 +757,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>35</v>
       </c>
@@ -779,7 +782,7 @@
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -790,7 +793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -801,7 +804,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -812,7 +815,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -823,7 +826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -834,7 +837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -845,7 +848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -856,7 +859,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -867,7 +870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -878,7 +881,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -889,7 +892,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -900,7 +903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -911,7 +914,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -922,7 +925,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -933,7 +936,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -942,6 +945,17 @@
       </c>
       <c r="D16" s="5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1555</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>